<commit_message>
Feature:	Further enhance User Guide and including templates for .xls format Files: 	PaiWei/Templates/e_pwTemplate.xls 	PaiWei/Templates/e_pwTemplate.xlsx 	PaiWei/Templates/pwTemplate.xls 	PaiWei/UG.php
</commit_message>
<xml_diff>
--- a/PaiWei/Templates/e_pwTemplate.xlsx
+++ b/PaiWei/Templates/e_pwTemplate.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berttan/MacPLC/admin/PaiWei/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C73A810-D120-4049-832E-C70899B36A39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8460764B-47FD-4443-B744-61D2DFC5A31D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="480" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="祈福消災" sheetId="1" r:id="rId1"/>
-    <sheet name="地基主牌位" sheetId="8" r:id="rId2"/>
-    <sheet name="歷代祖先牌位" sheetId="5" r:id="rId3"/>
-    <sheet name="往生親友牌位" sheetId="3" r:id="rId4"/>
-    <sheet name="累劫冤親債主牌位" sheetId="6" r:id="rId5"/>
-    <sheet name="12個月內往生親友牌位" sheetId="9" r:id="rId6"/>
+    <sheet name="Well Blessing" sheetId="1" r:id="rId1"/>
+    <sheet name="Site Guardian" sheetId="8" r:id="rId2"/>
+    <sheet name="Ancestors" sheetId="5" r:id="rId3"/>
+    <sheet name="Deceased" sheetId="3" r:id="rId4"/>
+    <sheet name="Karmic Creditors" sheetId="6" r:id="rId5"/>
+    <sheet name="Recently Deceased" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="W001A" localSheetId="5">'12個月內往生親友牌位'!$B$3:$F$522</definedName>
-    <definedName name="W001A" localSheetId="3">往生親友牌位!$B$3:$E$519</definedName>
+    <definedName name="W001A" localSheetId="3">Deceased!$B$3:$E$519</definedName>
+    <definedName name="W001A" localSheetId="5">'Recently Deceased'!$B$3:$F$522</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>

</xml_diff>